<commit_message>
# support nan values
</commit_message>
<xml_diff>
--- a/original_volentery_data.xlsx
+++ b/original_volentery_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaha\PycharmProjects\wordConventer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF2F8B-EDB9-4585-BAA6-94CCE11CF516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97882552-A7A7-435F-8A18-319B49D38D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Id</t>
   </si>
@@ -55,45 +55,18 @@
     <t>a7189bb6-87f5-4795-a968-cbc1518ba500</t>
   </si>
   <si>
-    <t>קרית אונו</t>
-  </si>
-  <si>
-    <t>15.9.2023, 19:58:40</t>
-  </si>
-  <si>
     <t>ec60cf1e-dee9-42c1-a36e-6c07a653c12b</t>
   </si>
   <si>
-    <t>15.9.2023, 19:28:47</t>
-  </si>
-  <si>
     <t>7437e6d8-a437-4046-b547-c2ecd3418fae</t>
   </si>
   <si>
-    <t>אלישמע</t>
-  </si>
-  <si>
-    <t>15.9.2023, 10:56:29</t>
-  </si>
-  <si>
     <t>b7245fa6-add0-4100-8592-4a085c548050</t>
   </si>
   <si>
-    <t>הרצליה</t>
-  </si>
-  <si>
-    <t>15.9.2023, 10:27:28</t>
-  </si>
-  <si>
     <t>9c51b954-a18a-40e8-bdc2-430aa166df64</t>
   </si>
   <si>
-    <t>רעננה</t>
-  </si>
-  <si>
-    <t>6.9.2023, 11:50:50</t>
-  </si>
-  <si>
     <t>שם פרטי ומשפחה</t>
   </si>
   <si>
@@ -148,34 +121,13 @@
     <t>עוגה בהפתעה</t>
   </si>
   <si>
-    <t>7.12.24</t>
-  </si>
-  <si>
-    <t>7.12.25</t>
-  </si>
-  <si>
-    <t>7.12.26</t>
-  </si>
-  <si>
-    <t>7.12.27</t>
-  </si>
-  <si>
-    <t>7.12.28</t>
-  </si>
-  <si>
-    <t>5.12.24</t>
-  </si>
-  <si>
-    <t>5.12.25</t>
-  </si>
-  <si>
-    <t>5.12.26</t>
-  </si>
-  <si>
-    <t>5.12.27</t>
-  </si>
-  <si>
-    <t>5.12.28</t>
+    <t>שחר שטוקהמר</t>
+  </si>
+  <si>
+    <t>כגדהדג</t>
+  </si>
+  <si>
+    <t>fgdfgdfg</t>
   </si>
 </sst>
 </file>
@@ -561,7 +513,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -569,7 +521,7 @@
     <col min="1" max="2" width="36.75" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="24.75" customWidth="1"/>
     <col min="4" max="4" width="23.25" customWidth="1"/>
-    <col min="5" max="5" width="24.75" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="32.75" customWidth="1"/>
     <col min="7" max="7" width="15.75" customWidth="1"/>
     <col min="8" max="8" width="13.75" customWidth="1"/>
@@ -588,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -597,40 +549,40 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="P1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -640,29 +592,47 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>318162112</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
       <c r="J2" t="s">
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
@@ -672,157 +642,37 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" t="s">
-        <v>47</v>
-      </c>
-      <c r="P4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" t="s">
-        <v>48</v>
-      </c>
-      <c r="P5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" t="s">
-        <v>49</v>
-      </c>
-      <c r="P6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" t="s">
-        <v>50</v>
-      </c>
-      <c r="P7" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -830,7 +680,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:B6 A1:B1 E1 J2:J6 J1 A7:B7 J7" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:B6 A1:B1 E1 J2 J1 A7:B7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>